<commit_message>
Add doc org section; updates Table 1
</commit_message>
<xml_diff>
--- a/tables/ProsCons2.xlsx
+++ b/tables/ProsCons2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KAlstad\Documents\Github_C\e-deviceIEP\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF546D6-0699-4139-BF1F-ABB83DC4C182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B01016-EF52-4A53-8773-A5CB7DAB0A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16335" yWindow="-16395" windowWidth="29040" windowHeight="15840" xr2:uid="{46186D46-7614-4C3B-A9CF-A71614DFEBF1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>Fulcrum</t>
   </si>
@@ -177,13 +177,6 @@
     <t>**Pros:** Provides user-friendly form building GUI that can be expanded/customized with Java coding.</t>
   </si>
   <si>
-    <t xml:space="preserve">**Cons:**  </t>
-  </si>
-  <si>
-    <t>**Pros:**  Can connect to external sensors; uses local area network 
---- --- --- ---</t>
-  </si>
-  <si>
     <t>**Pros:** Provides API potential for custom data interface with external sensors
 --- --- --- ---
 **Cons:**  Cannot read in data from local drive; No built in tool for connecting to sensors directly</t>
@@ -207,6 +200,9 @@
     <t>**Pros:** R-based PDF scraped data could be further processed in R
 --- --- --- ---
 **Cons:** All data configuratons must be coded by scratch requiring programming skills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Pros:**  Can connect to external sensors; uses local area network </t>
   </si>
 </sst>
 </file>
@@ -563,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E2A9D85-F5DE-46AF-938B-1B8F725A2C31}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,16 +674,16 @@
         <v>42</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>28</v>
@@ -704,7 +700,7 @@
         <v>41</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>16</v>
@@ -723,9 +719,6 @@
       <c r="B7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="D7" s="1" t="s">
         <v>22</v>
       </c>
@@ -744,7 +737,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>18</v>

</xml_diff>